<commit_message>
menambahkan create melalui kalender pada scheduling dan merapihkan import journal entry
</commit_message>
<xml_diff>
--- a/public/template/journal_entry_import_template.xlsx
+++ b/public/template/journal_entry_import_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\laporan_keuangan\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D46881E-D83F-4C87-A2B6-38507CEFC755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9DB3AE-CA05-4227-B370-AB7FEF785E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>source</t>
   </si>
@@ -37,45 +37,47 @@
     <t>kredit</t>
   </si>
   <si>
-    <t>manual</t>
-  </si>
-  <si>
-    <t>2025-07-01</t>
-  </si>
-  <si>
-    <t>Pembelian barang</t>
-  </si>
-  <si>
-    <t>11001</t>
-  </si>
-  <si>
-    <t>21001</t>
-  </si>
-  <si>
-    <t>bank</t>
-  </si>
-  <si>
-    <t>2025-07-02</t>
-  </si>
-  <si>
-    <t>Pembayaran hutang</t>
-  </si>
-  <si>
-    <t>12002</t>
-  </si>
-  <si>
-    <t>22002</t>
-  </si>
-  <si>
     <t>comment_line</t>
+  </si>
+  <si>
+    <t>departemen</t>
+  </si>
+  <si>
+    <t>nama_akun</t>
+  </si>
+  <si>
+    <t>MDR0012-2501-0001</t>
+  </si>
+  <si>
+    <t>2025-01-09</t>
+  </si>
+  <si>
+    <t>saldo qris MCM InhouseTrf DARI REMBULAN CITRA ABADI Transfer Fee 20250108193450725499102 — MDR0012-2501-0001 / 0001</t>
+  </si>
+  <si>
+    <t>ODS</t>
+  </si>
+  <si>
+    <t>1102002</t>
+  </si>
+  <si>
+    <t>1102001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -91,7 +93,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -99,12 +101,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,112 +427,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>1000000</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="E2">
-        <v>100000</v>
-      </c>
-      <c r="F2">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>130000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>150000</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>150000</v>
+      <c r="H3">
+        <v>1000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
menambahkan import dan export untuk beberapa menu
</commit_message>
<xml_diff>
--- a/public/template/journal_entry_import_template.xlsx
+++ b/public/template/journal_entry_import_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\laporan_keuangan\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9DB3AE-CA05-4227-B370-AB7FEF785E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCC53F5-9432-4FC7-8BCD-AE0AADF94526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,17 +58,17 @@
     <t>ODS</t>
   </si>
   <si>
-    <t>1102002</t>
-  </si>
-  <si>
-    <t>1102001</t>
+    <t>MANDIRI 1310000650012_QRIS ODS</t>
+  </si>
+  <si>
+    <t>MANDIRI 1310062136215_OPERASIONAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,13 +84,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F2937"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF4B5563"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9FAFB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -120,11 +138,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,10 +455,19 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="110.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -474,10 +508,10 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <v>1000000</v>
       </c>
       <c r="H2">
@@ -497,12 +531,10 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
+      <c r="G3" s="3"/>
       <c r="H3">
         <v>1000000</v>
       </c>

</xml_diff>

<commit_message>
menambahkan project pada journal entry
</commit_message>
<xml_diff>
--- a/public/template/journal_entry_import_template.xlsx
+++ b/public/template/journal_entry_import_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\laporan_keuangan\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCC53F5-9432-4FC7-8BCD-AE0AADF94526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBAD9D6-902E-4C17-81E8-F2B31AD72E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>source</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>MANDIRI 1310062136215_OPERASIONAL</t>
+  </si>
+  <si>
+    <t>project</t>
   </si>
 </sst>
 </file>
@@ -111,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -134,11 +137,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -150,6 +164,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,7 +486,7 @@
     <col min="7" max="8" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,8 +511,11 @@
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="I1" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -518,7 +538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
perbaikan template import journal entry
</commit_message>
<xml_diff>
--- a/public/template/journal_entry_import_template.xlsx
+++ b/public/template/journal_entry_import_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\laporan_keuangan\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBAD9D6-902E-4C17-81E8-F2B31AD72E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26FC4DA-7E04-4EDB-987D-97AC24E90957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
     <t>MANDIRI 1310062136215_OPERASIONAL</t>
   </si>
   <si>
-    <t>project</t>
+    <t>specpose</t>
   </si>
 </sst>
 </file>
@@ -164,7 +164,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>

</xml_diff>